<commit_message>
Fixed qualifier and region tutorial (added tag)
</commit_message>
<xml_diff>
--- a/tutorial/Region_Tutorial/region.xlsx
+++ b/tutorial/Region_Tutorial/region.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\t2wml\tutorial\region\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\t2wml\tutorial\Region_Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="00_region" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="39">
   <si>
     <t>dataset</t>
   </si>
@@ -136,16 +136,36 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>Tutorial dataset title</t>
+  </si>
+  <si>
+    <t>This is a description for the datatest used in the tutorial</t>
+  </si>
+  <si>
+    <t>https://github.com/usc-isi-i2/t2wml/tree/master/tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,13 +188,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,21 +500,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -505,7 +539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -519,81 +553,91 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -655,159 +699,150 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="A7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>123120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>123120</v>
+        <v>123125</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="E18">
-        <v>641254</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -815,12 +850,26 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D19">
+        <v>90</v>
+      </c>
+      <c r="E19">
+        <v>641254</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
         <v>50</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>246368</v>
       </c>
     </row>
@@ -831,9 +880,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -896,160 +947,165 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
       </c>
       <c r="F9">
-        <v>123120</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
       </c>
       <c r="F11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>31</v>
       </c>
       <c r="F13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <v>123125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>123120</v>
       </c>
     </row>
@@ -1060,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,133 +1183,138 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>123120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
+      <c r="D12">
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
         <v>123120</v>
       </c>
     </row>
@@ -1264,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,133 +1392,138 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>123120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
+      <c r="D12">
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
         <v>123120</v>
       </c>
     </row>
@@ -1468,9 +1534,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1527,106 +1595,111 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
         <v>25</v>
       </c>
     </row>
@@ -1637,9 +1710,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1702,133 +1777,138 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>123120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>123125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
         <v>123120</v>
       </c>
     </row>
@@ -1839,9 +1919,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1903,149 +1985,154 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="A7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>123120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>123120</v>
+        <v>123125</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>123120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2056,9 +2143,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2120,149 +2209,154 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="A7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>123120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>123120</v>
+        <v>123125</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>123120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2273,9 +2367,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2337,159 +2433,150 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="A7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>123120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17">
-        <v>123120</v>
+        <v>123125</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="E18">
-        <v>641254</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -2497,12 +2584,26 @@
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D19">
+        <v>90</v>
+      </c>
+      <c r="E19">
+        <v>641254</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
         <v>50</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>246368</v>
       </c>
     </row>
@@ -2513,9 +2614,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2578,160 +2681,165 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
       </c>
       <c r="F9">
-        <v>123120</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
       </c>
       <c r="F11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>31</v>
       </c>
       <c r="F13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <v>123125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>123120</v>
       </c>
     </row>
@@ -2742,9 +2850,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2807,133 +2917,138 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>123120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
+      <c r="D12">
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>123125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
         <v>123120</v>
       </c>
     </row>
@@ -2944,9 +3059,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3009,133 +3126,138 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
         <v>150000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>123120</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>122000</v>
+        <v>123120</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>123011</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
+      <c r="D12">
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>123123</v>
+        <v>123011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>123125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>123125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
         <v>123120</v>
       </c>
     </row>

</xml_diff>